<commit_message>
added the test with the ExcelUtils and DataProviderUtils
</commit_message>
<xml_diff>
--- a/testData/petStoreData.xlsx
+++ b/testData/petStoreData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/techglobal/IdeaProjects/backend-automation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D0DD84-DEE0-1C42-8D4F-8C435F187172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF141E0-DEF7-D54D-BE53-F43F3FFE053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="3460" windowWidth="38400" windowHeight="19960" xr2:uid="{D20F1619-F1A0-DE45-B693-13AAD6387145}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>